<commit_message>
feat: retrieve book data from Google Books API
</commit_message>
<xml_diff>
--- a/server/bookdata.xlsx
+++ b/server/bookdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A03235-5E31-4BB7-8816-F580165CF078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18710011-C9F3-4076-9408-A9D6EE5957A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{24C0A627-FD56-4D69-AC7F-3755FC5CBFF2}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{C3A5F0DE-22C1-4D78-909C-F059FAF4E3C8}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -755,7 +755,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="A33" sqref="A33:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fix: retrieve image links from Google Books API
</commit_message>
<xml_diff>
--- a/server/bookdata.xlsx
+++ b/server/bookdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18710011-C9F3-4076-9408-A9D6EE5957A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6913A6AA-0CD7-4114-9E6E-FBD8C3A67546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="139">
   <si>
     <t>id</t>
   </si>
@@ -428,6 +428,72 @@
   </si>
   <si>
     <t>31 Daughter of the Moon Goddess.jpg</t>
+  </si>
+  <si>
+    <t>Disney War</t>
+  </si>
+  <si>
+    <t>"When You Wish Upon a Star," "Whistle While You Work," "The Happiest Place on Earth" -- these are lyrics indelibly linked to Disney, one of the most admired and best-known companies in the world. So when Roy Disney, chairman of Walt Disney Animation and nephew of founder Walt Disney, abruptly resigned in November 2003 and declared war on chairman and chief executive Michael Eisner, he sent shock waves through the entertainment industry, corporate boardrooms, theme parks, and living rooms around the world -- everywhere Disney does business and its products are cherished.
+"DisneyWar" is the breathtaking, dramatic inside story of what drove America's best-known entertainment company to civil war, told by one of our most acclaimed writers and reporters.
+Drawing on unprecedented access to both Eisner and Roy Disney, current and former Disney executives and board members, as well as thousands of pages of never-before-seen letters, memos, transcripts, and other documents, James B. Stewart gets to the bottom of mysteries that have enveloped Disney for years: What really caused the rupture with studio chairman Jeffrey Katzenberg, a man who once regarded Eisner as a father but who became his fiercest rival? How could Eisner have so misjudged Michael Ovitz, a man who was not only "the most powerful man in Hollywood" but also his friend, whom he appointed as Disney president and immediately wanted to fire? What caused the break between Eisner and Pixar chairman Steve Jobs, and why did Pixar abruptly abandon its partnership with Disney? Why did Eisner so mistrust Roy Disney that he assigned Disney company executives to spy on him? How did Eisner control the Disney board for so long, and whatreally happened in the fateful board meeting in September 2004, when Eisner played his last cards?
+Here, too, is the creative process that lies at the heart of Disney -- from the making of "The Lion King" to "Pirates of the Caribbean." Even as the executive suite has been engulfed in turmoil, Disney has worked -- and sometimes clashed -- with a glittering array of stars, directors, designers, artists, and producers, many of whom tell their stories here for the first time.
+Stewart describes how Eisner lost his chairmanship and why he felt obliged to resign as CEO, effective 2006. No other book so thoroughly penetrates the secretive world of the corporate boardroom. "DisneyWar" is an enthralling tale of one of America's most powerful media and entertainment companies, the people who control it, and those trying to overthrow them.
+"DisneyWar" is an epic achievement. It tells a story that -- in its sudden twists, vivid, larger-than-life characters, and thrilling climax -- might itself have been the subject of a Disney animated classic -- except that it's all true.</t>
+  </si>
+  <si>
+    <t>32 Disney War.jpg</t>
+  </si>
+  <si>
+    <t>The Defense</t>
+  </si>
+  <si>
+    <t>Steve Cavanagh</t>
+  </si>
+  <si>
+    <t>Eddie Flynn used to be a con artist. Then he became a lawyer. Turns out the two jobs aren’t all that different. . .
+He vowed never to set foot in a courtroom again after a case gone disastrously wrong. But today Eddie doesn’t have a choice. Because this time, it’s personal.
+The head of the Russian mob in New York City, on trial for murder, has kidnapped Eddie’s beloved ten-year-old daughter. Now Eddie has exactly forty-eight hours to draw upon his razor-sharp instincts and use every con, bluff, grift, and trick in the book to defend an impossible trial and save his daughter—or die trying. . .</t>
+  </si>
+  <si>
+    <t>33 The Defense.jpg</t>
+  </si>
+  <si>
+    <t>Bad Blood: Secrets and Lies in a Silicon Valley Startup</t>
+  </si>
+  <si>
+    <t>John Carreyrou</t>
+  </si>
+  <si>
+    <t>The gripping story of Elizabeth Holmes and Theranos—one of the biggest corporate frauds in history—a tale of ambition and hubris set amid the bold promises of Silicon Valley, rigorously reported by the prize-winning journalist. With a new Afterword covering her trial and sentencing, bringing the story to a close.
+In 2014, Theranos founder and CEO Elizabeth Holmes was widely seen as the next Steve Jobs: a brilliant Stanford dropout whose startup “unicorn” promised to revolutionize the medical industry with its breakthrough device, which performed the whole range of laboratory tests from a single drop of blood. Backed by investors such as Larry Ellison and Tim Draper, Theranos sold shares in a fundraising round that valued the company at more than $9 billion, putting Holmes’s worth at an estimated $4.5 billion. There was just one problem: The technology didn’t work. Erroneous results put patients in danger, leading to misdiagnoses and unnecessary treatments. All the while, Holmes and her partner, Sunny Balwani, worked to silence anyone who voiced misgivings—from journalists to their own employees.</t>
+  </si>
+  <si>
+    <t>34 Bad Blood.jpg</t>
+  </si>
+  <si>
+    <t>The Thursday Murder Club</t>
+  </si>
+  <si>
+    <t>Richard Osman</t>
+  </si>
+  <si>
+    <t>In a peaceful retirement village, four unlikely friends meet weekly in the Jigsaw Room to discuss unsolved crimes; together they call themselves the Thursday Murder Club.
+When a local developer is found dead with a mysterious photograph left next to the body, the Thursday Murder Club suddenly find themselves in the middle of their first live case.
+As the bodies begin to pile up, can our unorthodox but brilliant gang catch the killer, before it's too late?</t>
+  </si>
+  <si>
+    <t>35 The Thursday Murder Club.jpg</t>
+  </si>
+  <si>
+    <t>Lord Edgware Dies</t>
+  </si>
+  <si>
+    <t>In this official authorized edition from the Queen of Mystery, detective Hercule Poirot must solve a most confounding conundrum when Lord Edgware has a most unnatural death.
+When Lord Edgware is found murdered the police are baffled. His estranged actress wife was seen visiting him just before his death and Hercule Poirot himself heard her brag of her plan to "get rid" of him.
+But how could she have stabbed Lord Edgware in his library at exactly the same time she was seen dining with friends? It's a case that almost proves to be too much for the great Poirot.</t>
+  </si>
+  <si>
+    <t>36 Lord Edgware Dies.jpg</t>
   </si>
 </sst>
 </file>
@@ -476,7 +542,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{C3A5F0DE-22C1-4D78-909C-F059FAF4E3C8}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{E76CBAFB-1CA6-46DB-95FE-E87EFC1DB4C9}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -752,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1434,6 +1500,106 @@
         <v>45564.926246261573</v>
       </c>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="3">
+        <v>45575.967919884264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" s="3">
+        <v>45578.26440537037</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" s="3">
+        <v>45584.20642707176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" t="s">
+        <v>135</v>
+      </c>
+      <c r="F36" s="3">
+        <v>45586.123904548615</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>137</v>
+      </c>
+      <c r="E37" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" s="3">
+        <v>45589.084046307871</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: save genre data
</commit_message>
<xml_diff>
--- a/server/bookdata.xlsx
+++ b/server/bookdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6913A6AA-0CD7-4114-9E6E-FBD8C3A67546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D218C7-B95C-49ED-AC45-977A894FEFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="182">
   <si>
     <t>id</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>genres</t>
   </si>
   <si>
     <t>The Power of Habit: Why We Do What We Do in Life and Business</t>
@@ -60,6 +63,12 @@
   </si>
   <si>
     <t>1 The Power of Habit.jpg</t>
+  </si>
+  <si>
+    <t>Nonfiction</t>
+  </si>
+  <si>
+    <t>Business &amp; Economics / Organizational Behavior / Psychology / Social Psychology / Self-Help / Personal Growth / General</t>
   </si>
   <si>
     <t>All My Rage</t>
@@ -80,6 +89,12 @@
     <t>2 All My Rage.jpg</t>
   </si>
   <si>
+    <t>Fiction</t>
+  </si>
+  <si>
+    <t>Young Adult Fiction / Family / Multigenerational / General / Juvenile Fiction</t>
+  </si>
+  <si>
     <t>Smoke Gets in Your Eyes &amp; Other Lessons from the Crematory</t>
   </si>
   <si>
@@ -96,6 +111,9 @@
     <t>3 Smoke Gets in Your Eyes.jpg</t>
   </si>
   <si>
+    <t>Biography &amp; Autobiography / Personal Memoirs / Medical / Forensic Medicine / Self-Help / Death, Grief, Bereavement / Social Science / Death &amp; Dying</t>
+  </si>
+  <si>
     <t>From Here to Eternity</t>
   </si>
   <si>
@@ -105,6 +123,9 @@
     <t>4 From Here to Eternity.jpg</t>
   </si>
   <si>
+    <t>Biography &amp; Autobiography / Personal Memoirs / Social Science / Death &amp; Dying / Travel / Essays &amp; Travelogues</t>
+  </si>
+  <si>
     <t>Sideways: The City Google Couldn't Buy</t>
   </si>
   <si>
@@ -117,6 +138,9 @@
     <t>5 Sideways.jpg</t>
   </si>
   <si>
+    <t>Business &amp; Economics / Industries / Computers &amp; Information Technology / Political Science / Public Policy / City Planning &amp; Urban Development / Urban &amp; Regional</t>
+  </si>
+  <si>
     <t>Invisible Women: Data Bias in a World Designed for Men</t>
   </si>
   <si>
@@ -129,6 +153,9 @@
     <t>6 Invisible Women.jpg</t>
   </si>
   <si>
+    <t>Computers / Social Aspects / Business &amp; Economics / Industries / Computers &amp; Information Technology / Social Science / Women's Studies / Political Science / Civil Rights / Technology &amp; Engineering</t>
+  </si>
+  <si>
     <t>This Time Tomorrow</t>
   </si>
   <si>
@@ -139,6 +166,9 @@
   </si>
   <si>
     <t>7 This Time Tomorrow.jpg</t>
+  </si>
+  <si>
+    <t>Fiction / Science Fiction / General / Time Travel / Women / Family Life</t>
   </si>
   <si>
     <t>Lady Killers: Deadly Women Throughout History</t>
@@ -156,6 +186,9 @@
     <t>8 Lady Killers.jpg</t>
   </si>
   <si>
+    <t>True Crime / Murder / Serial Killers / Historical / Social Science / Violence in Society / Women's Studies</t>
+  </si>
+  <si>
     <t>Lessons in Chemistry</t>
   </si>
   <si>
@@ -168,6 +201,9 @@
     <t>9 Lessons in Chemistry.jpg</t>
   </si>
   <si>
+    <t>Fiction / Feminist / Women / Literary</t>
+  </si>
+  <si>
     <t>Why Flying is Miserable and How to Fix it</t>
   </si>
   <si>
@@ -180,6 +216,9 @@
     <t>10 Why Flying is Miserable.jpg</t>
   </si>
   <si>
+    <t>Business &amp; Economics / General / Industries / Transportation / Corporate &amp; Business History / Hospitality, Travel &amp; Tourism / Travel</t>
+  </si>
+  <si>
     <t>Inflamed: Deep Medicine and the Anatomy of Injustice</t>
   </si>
   <si>
@@ -192,6 +231,9 @@
     <t>11 Inflamed.jpg</t>
   </si>
   <si>
+    <t>Social Science / Disease &amp; Health Issues / Medical / Healing / Political Science / Public Policy / Health Care / Public Health</t>
+  </si>
+  <si>
     <t>Murder on the Orient Express</t>
   </si>
   <si>
@@ -202,6 +244,9 @@
   </si>
   <si>
     <t>12 Murder on the Orient Express.jpg</t>
+  </si>
+  <si>
+    <t>Fiction / Mystery &amp; Detective / General / Traditional / Thrillers / Crime / Family Life / Amateur Sleuth / Classics</t>
   </si>
   <si>
     <t>The Mysterious Affair at Styles</t>
@@ -217,6 +262,9 @@
     <t>13 The Mysterious Affair at Styles.jpg</t>
   </si>
   <si>
+    <t>Fiction / Classics / Mystery &amp; Detective / Private Investigators / Literary</t>
+  </si>
+  <si>
     <t>The Murder on the Links</t>
   </si>
   <si>
@@ -226,6 +274,9 @@
     <t>14 The Murder on the Links.jpg</t>
   </si>
   <si>
+    <t>Fiction / Mystery &amp; Detective / General</t>
+  </si>
+  <si>
     <t>The Lonely Hearts Book Club</t>
   </si>
   <si>
@@ -236,6 +287,9 @@
   </si>
   <si>
     <t>15 The Lonely Hearts Book Club.jpg</t>
+  </si>
+  <si>
+    <t>Fiction / Women / Friendship / Small Town &amp; Rural / Coming of Age / Literary</t>
   </si>
   <si>
     <t xml:space="preserve">I'll Be Gone in the Dark: One Woman's Obsessive Search for the Golden State Killer </t>
@@ -252,6 +306,9 @@
     <t>16 I'll Be Gone in the Dark.jpg</t>
   </si>
   <si>
+    <t>True Crime / Murder / Serial Killers / Biography &amp; Autobiography / Personal Memoirs / Law Enforcement / History / Essays / Historical / Law / Criminal Law / General / Criminals &amp; Outlaws / North America / Americas (North, Central, South, West Indies)</t>
+  </si>
+  <si>
     <t>And Then There Were None</t>
   </si>
   <si>
@@ -261,6 +318,9 @@
     <t>17 And Then There Were None.jpg</t>
   </si>
   <si>
+    <t>Fiction / Mystery &amp; Detective / Traditional / Crime / Historical / General</t>
+  </si>
+  <si>
     <t>The Murder of Roger Ackroyd</t>
   </si>
   <si>
@@ -268,6 +328,9 @@
   </si>
   <si>
     <t>18 The Murder of Roger Ackroyd.jpg</t>
+  </si>
+  <si>
+    <t>Fiction / Mystery &amp; Detective / Traditional / Classics / Thrillers / Crime</t>
   </si>
   <si>
     <t>Magpie Murders</t>
@@ -285,6 +348,9 @@
     <t>19 Magpie Murders.jpg</t>
   </si>
   <si>
+    <t>Fiction / Mystery &amp; Detective / Amateur Sleuth / General</t>
+  </si>
+  <si>
     <t>The Big Four</t>
   </si>
   <si>
@@ -310,6 +376,9 @@
     <t>21 Unscripted.jpg</t>
   </si>
   <si>
+    <t>Business &amp; Economics / Industries / Media &amp; Communications / Biography &amp; Autobiography / Entertainment &amp; Performing Arts / True Crime / Con Artists, Hoaxes &amp; Deceptions</t>
+  </si>
+  <si>
     <t>Mystery of the Blue Train</t>
   </si>
   <si>
@@ -321,6 +390,9 @@
     <t>22 The Mystery of the Blue Train.jpg</t>
   </si>
   <si>
+    <t>Fiction / Mystery &amp; Detective / Private Investigators / Traditional / General</t>
+  </si>
+  <si>
     <t>Found in a Bookshop</t>
   </si>
   <si>
@@ -333,6 +405,9 @@
     <t>23 Found in a Bookshop.jpg</t>
   </si>
   <si>
+    <t>Fiction / General / Literary / Romance / Women / Family Life / Friendship / Literary Criticism</t>
+  </si>
+  <si>
     <t>Battle of Ink and Ice</t>
   </si>
   <si>
@@ -345,6 +420,9 @@
     <t>24 Battle of Ink and Ice.jpg</t>
   </si>
   <si>
+    <t>History / Expeditions &amp; Discoveries / Social Science / Media Studies / United States / 20th Century</t>
+  </si>
+  <si>
     <t>Peril at End House</t>
   </si>
   <si>
@@ -364,6 +442,9 @@
   </si>
   <si>
     <t>26 Denison Avenue.jpg</t>
+  </si>
+  <si>
+    <t>Fiction / Asian American / City Life / Comics &amp; Graphic Novels / Literary</t>
   </si>
   <si>
     <t>Blind Eye: How the Medical Establishment Let a Doctor Get Away With Murder</t>
@@ -381,6 +462,9 @@
     <t>27 Blind Eye.jpg</t>
   </si>
   <si>
+    <t>Biography &amp; Autobiography / Medical (incl. Patients) / Current Events / General / Medical / Ethics / Physicians / Political Science / True Crime / Murder / Serial Killers</t>
+  </si>
+  <si>
     <t>A Study in Scarlet</t>
   </si>
   <si>
@@ -395,6 +479,9 @@
     <t>28 A Study in Scarlet.jpg</t>
   </si>
   <si>
+    <t>Fiction / Classics / Mystery &amp; Detective / Traditional / Historical</t>
+  </si>
+  <si>
     <t>The Girls We Sent Away</t>
   </si>
   <si>
@@ -405,6 +492,9 @@
   </si>
   <si>
     <t>29 The Girls We Sent Away.jpg</t>
+  </si>
+  <si>
+    <t>Fiction / Southern / Historical / General / Women / Small Town &amp; Rural / Literary</t>
   </si>
   <si>
     <t>Den of Thieves</t>
@@ -418,6 +508,9 @@
     <t>30 Den of Thieves.jpg</t>
   </si>
   <si>
+    <t>True Crime / White Collar Crime / Business &amp; Economics / Business Ethics / Banks &amp; Banking / General</t>
+  </si>
+  <si>
     <t>Daughter of the Moon Goddess</t>
   </si>
   <si>
@@ -428,6 +521,9 @@
   </si>
   <si>
     <t>31 Daughter of the Moon Goddess.jpg</t>
+  </si>
+  <si>
+    <t>Fiction / Fantasy / Romance / Epic / Fairy Tales, Folk Tales, Legends &amp; Mythology / Cultural Heritage / World Literature / China / General / Coming of Age / Action &amp; Adventure / Animals / Drama / American</t>
   </si>
   <si>
     <t>Disney War</t>
@@ -444,6 +540,9 @@
     <t>32 Disney War.jpg</t>
   </si>
   <si>
+    <t>Business &amp; Economics / Corporate &amp; Business History / Corporate Governance / Biography &amp; Autobiography / Business / Performing Arts / Film / General</t>
+  </si>
+  <si>
     <t>The Defense</t>
   </si>
   <si>
@@ -458,6 +557,9 @@
     <t>33 The Defense.jpg</t>
   </si>
   <si>
+    <t>Fiction / Thrillers / Legal / Suspense</t>
+  </si>
+  <si>
     <t>Bad Blood: Secrets and Lies in a Silicon Valley Startup</t>
   </si>
   <si>
@@ -469,6 +571,9 @@
   </si>
   <si>
     <t>34 Bad Blood.jpg</t>
+  </si>
+  <si>
+    <t>Business &amp; Economics / Entrepreneurship / Corporate Finance / Venture Capital / Technology &amp; Engineering / Biomedical</t>
   </si>
   <si>
     <t>The Thursday Murder Club</t>
@@ -485,6 +590,9 @@
     <t>35 The Thursday Murder Club.jpg</t>
   </si>
   <si>
+    <t>Fiction / Mystery &amp; Detective / Amateur Sleuth / General / Cozy</t>
+  </si>
+  <si>
     <t>Lord Edgware Dies</t>
   </si>
   <si>
@@ -494,6 +602,29 @@
   </si>
   <si>
     <t>36 Lord Edgware Dies.jpg</t>
+  </si>
+  <si>
+    <t>Fiction / Mystery &amp; Detective / Traditional / Thrillers / Crime / Family Life / General / Amateur Sleuth / Cozy / Classics / Historical</t>
+  </si>
+  <si>
+    <t>Some People Need Killing: A Memoir of Murder in My Country</t>
+  </si>
+  <si>
+    <t>Patricia Evangelista</t>
+  </si>
+  <si>
+    <t>For six years, journalist Patricia Evangelista documented killings carried out by police and vigilantes in the name of then president Rodrigo Duterte’s war on drugs—a crusade that led to the slaughter of thousands—immersing herself in the world of killers and survivors and capturing the atmosphere of terror created when an elected president decides that some lives are worth less than others.
+The book takes its title from the words of a vigilante, which demonstrated the psychological accommodation many across the country had made: “I’m really not a bad guy,” he said. “I’m not all bad. Some people need killing.”
+A profound act of witness and a tour de force of literary journalism, Some People Need Killing is a brilliant dissection of the grammar of violence and an investigation into the human impulses to dominate and resist.</t>
+  </si>
+  <si>
+    <t>37 Some People Need Killing.jpg</t>
+  </si>
+  <si>
+    <t>Political Science / World / Asian / History / Asia / Southeast Asia / Biography &amp; Autobiography / Editors, Journalists, Publishers</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -542,7 +673,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{E76CBAFB-1CA6-46DB-95FE-E87EFC1DB4C9}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{181C6C82-9BED-40CD-80F1-2232F946A4BD}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -818,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -834,7 +965,7 @@
     <col min="6" max="6" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,751 +984,999 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="101.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="101.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f t="shared" ref="A2:A4" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
         <v>44757</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3">
         <v>44771</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="174" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="174" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A25" si="1">ROW()-1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3">
         <v>45078</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F6" s="3">
         <v>45206</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F7" s="3">
         <v>45206</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F8" s="3">
         <v>45217</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F9" s="3">
         <v>45338</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F10" s="3">
         <v>45400</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F11" s="3">
         <v>45400</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F12" s="3">
         <v>45400</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F13" s="3">
         <v>45400</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="145" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="145" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F14" s="3">
         <v>45419</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F15" s="3">
         <v>45419</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="F16" s="3">
         <v>45419</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F17" s="3">
         <v>45434</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="F18" s="3">
         <v>45458</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="F19" s="3">
         <v>45458</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="F20" s="3">
         <v>45498</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="F21" s="3">
         <v>45498</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="116" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="116" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="F22" s="3">
         <v>45498</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="F23" s="3">
         <v>45498</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="F24" s="3">
         <v>45519</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="F25" s="3">
         <v>45519</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <f>ROW()-1</f>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="F26" s="3">
         <v>45523</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <f>ROW()-1</f>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="D27" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="F27" s="3">
         <v>45535</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="116" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="116" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="E28" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="F28" s="3">
         <v>45541</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="D29" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="F29" s="3">
         <v>45543</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="E30" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="F30" s="3">
         <v>45546</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="D31" t="s">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="F31" s="3">
         <v>45560</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="D32" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="E32" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="F32" s="3">
         <v>45564.926246261573</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="C33" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="E33" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="F33" s="3">
         <v>45575.967919884264</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="C34" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="D34" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
       <c r="E34" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="F34" s="3">
         <v>45578.26440537037</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="C35" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="D35" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="E35" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="F35" s="3">
         <v>45584.20642707176</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="D36" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="E36" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="F36" s="3">
         <v>45586.123904548615</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="F37" s="3">
         <v>45589.084046307871</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>176</v>
+      </c>
+      <c r="C38" t="s">
+        <v>177</v>
+      </c>
+      <c r="D38" t="s">
+        <v>178</v>
+      </c>
+      <c r="E38" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="3">
+        <v>45602.261537442129</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: display page count and genres
</commit_message>
<xml_diff>
--- a/server/bookdata.xlsx
+++ b/server/bookdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D218C7-B95C-49ED-AC45-977A894FEFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20EA2FA-BA00-4747-ACA2-3DE73226CE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="183">
   <si>
     <t>id</t>
   </si>
@@ -48,7 +48,13 @@
     <t>date</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
     <t>genres</t>
+  </si>
+  <si>
+    <t>pagecount</t>
   </si>
   <si>
     <t>The Power of Habit: Why We Do What We Do in Life and Business</t>
@@ -622,9 +628,6 @@
   </si>
   <si>
     <t>Political Science / World / Asian / History / Asia / Southeast Asia / Biography &amp; Autobiography / Editors, Journalists, Publishers</t>
-  </si>
-  <si>
-    <t>type</t>
   </si>
 </sst>
 </file>
@@ -673,7 +676,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{181C6C82-9BED-40CD-80F1-2232F946A4BD}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{9D3B2368-5302-4ACC-90B0-4D1B8584806A}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -949,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -963,9 +966,12 @@
     <col min="4" max="4" width="255.6328125" customWidth="1"/>
     <col min="5" max="5" width="31.90625" customWidth="1"/>
     <col min="6" max="6" width="10.08984375" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" customWidth="1"/>
+    <col min="8" max="8" width="26.08984375" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -985,998 +991,1112 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>181</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="101.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="101.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f t="shared" ref="A2:A4" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3">
         <v>44757</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3">
         <v>44771</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="174" customHeight="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="174" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3">
         <v>44788</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A25" si="1">ROW()-1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3">
         <v>45078</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="I5">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F6" s="3">
         <v>45206</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="I6">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F7" s="3">
         <v>45206</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I7">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F8" s="3">
         <v>45217</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="I8">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F9" s="3">
         <v>45338</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="I9">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F10" s="3">
         <v>45400</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="I10">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F11" s="3">
         <v>45400</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="I11">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3">
         <v>45400</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="I12">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F13" s="3">
         <v>45400</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="145" customHeight="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+      <c r="I13">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="145" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F14" s="3">
         <v>45419</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="I14">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F15" s="3">
         <v>45419</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="I15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F16" s="3">
         <v>45419</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+      <c r="I16">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F17" s="3">
         <v>45434</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+      <c r="I17">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F18" s="3">
         <v>45458</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+      <c r="I18">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F19" s="3">
         <v>45458</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+      <c r="I19">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F20" s="3">
         <v>45498</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="I20">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F21" s="3">
         <v>45498</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="116" customHeight="1" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="I21">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="116" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F22" s="3">
         <v>45498</v>
       </c>
       <c r="G22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+      <c r="I22">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F23" s="3">
         <v>45498</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+      <c r="I23">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F24" s="3">
         <v>45519</v>
       </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+      <c r="I24">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E25" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F25" s="3">
         <v>45519</v>
       </c>
       <c r="G25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+      <c r="I25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <f>ROW()-1</f>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F26" s="3">
         <v>45523</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+      <c r="I26">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <f>ROW()-1</f>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F27" s="3">
         <v>45535</v>
       </c>
       <c r="G27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="116" customHeight="1" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+      <c r="I27">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="116" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E28" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F28" s="3">
         <v>45541</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+      <c r="I28">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D29" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E29" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F29" s="3">
         <v>45543</v>
       </c>
       <c r="G29" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H29" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+      <c r="I29">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C30" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F30" s="3">
         <v>45546</v>
       </c>
       <c r="G30" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H30" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+      <c r="I30">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E31" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F31" s="3">
         <v>45560</v>
       </c>
       <c r="G31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H31" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+      <c r="I31">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D32" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E32" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F32" s="3">
         <v>45564.926246261573</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+      <c r="I32">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E33" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F33" s="3">
         <v>45575.967919884264</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H33" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+      <c r="I33">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E34" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F34" s="3">
         <v>45578.26440537037</v>
       </c>
       <c r="G34" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+      <c r="I34">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D35" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E35" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F35" s="3">
         <v>45584.20642707176</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H35" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="I35">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D36" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F36" s="3">
         <v>45586.123904548615</v>
       </c>
       <c r="G36" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H36" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+      <c r="I36">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E37" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F37" s="3">
         <v>45589.084046307871</v>
       </c>
       <c r="G37" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+      <c r="I37">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C38" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D38" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E38" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F38" s="3">
         <v>45602.261537442129</v>
       </c>
       <c r="G38" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H38" t="s">
-        <v>180</v>
+        <v>182</v>
+      </c>
+      <c r="I38">
+        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>